<commit_message>
Update edited session - 2025-12-30T13:19:46.050Z - Cache Bust ID: 1767100786050w4nxximha
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Cardiology_scanner1767098921465_897d3d4ed4cd1629116f10f67f18ed4532b1b68fb7fd145e360e1c8b876713b0.xlsx
+++ b/log_history/Y4_B2526_Cardiology_scanner1767098921465_897d3d4ed4cd1629116f10f67f18ed4532b1b68fb7fd145e360e1c8b876713b0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Cardiology" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>211631</v>
+        <v>211590</v>
       </c>
       <c r="B31" t="str">
         <v>Cardiology</v>
@@ -1013,7 +1013,7 @@
         <v>30/12/2025</v>
       </c>
       <c r="D31" t="str">
-        <v>15:13:46</v>
+        <v>15:13:55</v>
       </c>
       <c r="E31" t="str">
         <v>Manual</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>211590</v>
+        <v>211643</v>
       </c>
       <c r="B32" t="str">
         <v>Cardiology</v>
@@ -1033,7 +1033,7 @@
         <v>30/12/2025</v>
       </c>
       <c r="D32" t="str">
-        <v>15:13:55</v>
+        <v>15:14:07</v>
       </c>
       <c r="E32" t="str">
         <v>Manual</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>211643</v>
+        <v>211197</v>
       </c>
       <c r="B33" t="str">
         <v>Cardiology</v>
@@ -1053,7 +1053,7 @@
         <v>30/12/2025</v>
       </c>
       <c r="D33" t="str">
-        <v>15:14:07</v>
+        <v>15:14:17</v>
       </c>
       <c r="E33" t="str">
         <v>Manual</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>211197</v>
+        <v>211175</v>
       </c>
       <c r="B34" t="str">
         <v>Cardiology</v>
@@ -1073,7 +1073,7 @@
         <v>30/12/2025</v>
       </c>
       <c r="D34" t="str">
-        <v>15:14:17</v>
+        <v>15:14:27</v>
       </c>
       <c r="E34" t="str">
         <v>Manual</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>211217</v>
+        <v>211086</v>
       </c>
       <c r="B35" t="str">
         <v>Cardiology</v>
@@ -1093,7 +1093,7 @@
         <v>30/12/2025</v>
       </c>
       <c r="D35" t="str">
-        <v>15:14:21</v>
+        <v>15:14:34</v>
       </c>
       <c r="E35" t="str">
         <v>Manual</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>211175</v>
+        <v>211111</v>
       </c>
       <c r="B36" t="str">
         <v>Cardiology</v>
@@ -1113,7 +1113,7 @@
         <v>30/12/2025</v>
       </c>
       <c r="D36" t="str">
-        <v>15:14:27</v>
+        <v>15:14:53</v>
       </c>
       <c r="E36" t="str">
         <v>Manual</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>211086</v>
+        <v>211299</v>
       </c>
       <c r="B37" t="str">
         <v>Cardiology</v>
@@ -1133,7 +1133,7 @@
         <v>30/12/2025</v>
       </c>
       <c r="D37" t="str">
-        <v>15:14:34</v>
+        <v>15:15:01</v>
       </c>
       <c r="E37" t="str">
         <v>Manual</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>211111</v>
+        <v>211298</v>
       </c>
       <c r="B38" t="str">
         <v>Cardiology</v>
@@ -1153,7 +1153,7 @@
         <v>30/12/2025</v>
       </c>
       <c r="D38" t="str">
-        <v>15:14:53</v>
+        <v>15:15:06</v>
       </c>
       <c r="E38" t="str">
         <v>Manual</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>211299</v>
+        <v>211267</v>
       </c>
       <c r="B39" t="str">
         <v>Cardiology</v>
@@ -1173,7 +1173,7 @@
         <v>30/12/2025</v>
       </c>
       <c r="D39" t="str">
-        <v>15:15:01</v>
+        <v>15:15:13</v>
       </c>
       <c r="E39" t="str">
         <v>Manual</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>211298</v>
+        <v>211263</v>
       </c>
       <c r="B40" t="str">
         <v>Cardiology</v>
@@ -1193,7 +1193,7 @@
         <v>30/12/2025</v>
       </c>
       <c r="D40" t="str">
-        <v>15:15:06</v>
+        <v>15:16:04</v>
       </c>
       <c r="E40" t="str">
         <v>Manual</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>211267</v>
+        <v>211637</v>
       </c>
       <c r="B41" t="str">
         <v>Cardiology</v>
@@ -1213,58 +1213,18 @@
         <v>30/12/2025</v>
       </c>
       <c r="D41" t="str">
-        <v>15:15:13</v>
+        <v>15:16:14</v>
       </c>
       <c r="E41" t="str">
         <v>Manual</v>
       </c>
       <c r="F41" t="str">
-        <v>drmohamedramadan50@gmail.com</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="str">
-        <v>211263</v>
-      </c>
-      <c r="B42" t="str">
-        <v>Cardiology</v>
-      </c>
-      <c r="C42" t="str">
-        <v>30/12/2025</v>
-      </c>
-      <c r="D42" t="str">
-        <v>15:16:04</v>
-      </c>
-      <c r="E42" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F42" t="str">
-        <v>drmohamedramadan50@gmail.com</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="str">
-        <v>211637</v>
-      </c>
-      <c r="B43" t="str">
-        <v>Cardiology</v>
-      </c>
-      <c r="C43" t="str">
-        <v>30/12/2025</v>
-      </c>
-      <c r="D43" t="str">
-        <v>15:16:14</v>
-      </c>
-      <c r="E43" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F43" t="str">
         <v>drmohamedramadan50@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F43"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F41"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>